<commit_message>
- Para evitar bugs, todos os acentos foram retirados do codigo e do banco dados_organizados - organizacao de codigos enviados dia 08/06 que possivelmente nao serao utilizados - insercao de codigos "Modelagem" enviados dia 20/06 e organizacao ate a modelagem do estagio I. Aparentemente o codigo abaixo e analogo.
</commit_message>
<xml_diff>
--- a/dados_organizados.xlsx
+++ b/dados_organizados.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yugo\Academico\IME\2021-1\MAE0413 - Estatística Aplicada I\Projeto\R\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yugo\Academico\IME\2021-1\MAE0413 - Estatistica Aplicada I\Projeto\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC162BEE-D1A6-4932-8EB1-1B3EA28A9DA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC730A5A-7739-489B-A14E-4EF2CDAAE23D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="3510" windowWidth="20640" windowHeight="11760" xr2:uid="{B4BAF989-F6DA-4466-A9B7-8C14BC79726F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B4BAF989-F6DA-4466-A9B7-8C14BC79726F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -34,18 +34,6 @@
   </si>
   <si>
     <t>amostra nº</t>
-  </si>
-  <si>
-    <t>Estágio I</t>
-  </si>
-  <si>
-    <t>Estágio II</t>
-  </si>
-  <si>
-    <t>Estágio III</t>
-  </si>
-  <si>
-    <t>Estágio IV</t>
   </si>
   <si>
     <t>oviduto</t>
@@ -79,6 +67,18 @@
   </si>
   <si>
     <t>femea</t>
+  </si>
+  <si>
+    <t>Estagio I</t>
+  </si>
+  <si>
+    <t>Estagio II</t>
+  </si>
+  <si>
+    <t>Estagio III</t>
+  </si>
+  <si>
+    <t>Estagio IV</t>
   </si>
 </sst>
 </file>
@@ -529,7 +529,7 @@
   <dimension ref="A1:J91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -547,7 +547,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -556,25 +556,25 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="H1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="I1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
@@ -1001,7 +1001,7 @@
     </row>
     <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B17" s="2">
         <v>40238</v>
@@ -1031,7 +1031,7 @@
     </row>
     <row r="18" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B18" s="2">
         <v>40281</v>
@@ -1061,7 +1061,7 @@
     </row>
     <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B19" s="2">
         <v>40316</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="20" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B20" s="2">
         <v>40345</v>
@@ -1121,7 +1121,7 @@
     </row>
     <row r="21" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B21" s="2">
         <v>40403</v>
@@ -1151,7 +1151,7 @@
     </row>
     <row r="22" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B22" s="2">
         <v>40437</v>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="23" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B23" s="2">
         <v>40465</v>
@@ -1215,7 +1215,7 @@
     </row>
     <row r="24" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B24" s="2">
         <v>40527</v>
@@ -1241,7 +1241,7 @@
     </row>
     <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B25" s="2">
         <v>40549</v>
@@ -1271,7 +1271,7 @@
     </row>
     <row r="26" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B26" s="2">
         <v>40598</v>
@@ -1301,7 +1301,7 @@
     </row>
     <row r="27" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B27" s="2">
         <v>40659</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B28" s="2">
         <v>40723</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B29" s="2">
         <v>40779</v>
@@ -1391,7 +1391,7 @@
     </row>
     <row r="30" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B30" s="2">
         <v>40848</v>
@@ -1413,7 +1413,7 @@
     </row>
     <row r="31" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B31" s="2">
         <v>40864</v>
@@ -1429,7 +1429,7 @@
     </row>
     <row r="32" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B32" s="2">
         <v>40238</v>
@@ -1459,7 +1459,7 @@
     </row>
     <row r="33" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B33" s="2">
         <v>40281</v>
@@ -1489,7 +1489,7 @@
     </row>
     <row r="34" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B34" s="2">
         <v>40316</v>
@@ -1519,7 +1519,7 @@
     </row>
     <row r="35" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B35" s="2">
         <v>40345</v>
@@ -1549,7 +1549,7 @@
     </row>
     <row r="36" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B36" s="2">
         <v>40403</v>
@@ -1573,7 +1573,7 @@
     </row>
     <row r="37" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B37" s="2">
         <v>40437</v>
@@ -1603,7 +1603,7 @@
     </row>
     <row r="38" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B38" s="2">
         <v>40465</v>
@@ -1633,7 +1633,7 @@
     </row>
     <row r="39" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B39" s="2">
         <v>40527</v>
@@ -1663,7 +1663,7 @@
     </row>
     <row r="40" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B40" s="2">
         <v>40549</v>
@@ -1693,7 +1693,7 @@
     </row>
     <row r="41" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B41" s="2">
         <v>40598</v>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="42" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B42" s="2">
         <v>40659</v>
@@ -1753,7 +1753,7 @@
     </row>
     <row r="43" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B43" s="2">
         <v>40723</v>
@@ -1783,7 +1783,7 @@
     </row>
     <row r="44" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B44" s="2">
         <v>40779</v>
@@ -1808,12 +1808,12 @@
       </c>
       <c r="I44" s="9"/>
       <c r="J44" s="9" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B45" s="2">
         <v>40848</v>
@@ -1835,7 +1835,7 @@
     </row>
     <row r="46" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B46" s="2">
         <v>40864</v>
@@ -1851,7 +1851,7 @@
     </row>
     <row r="47" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B47" s="2">
         <v>40238</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="48" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B48" s="2">
         <v>40281</v>
@@ -1911,7 +1911,7 @@
     </row>
     <row r="49" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B49" s="2">
         <v>40316</v>
@@ -1941,7 +1941,7 @@
     </row>
     <row r="50" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B50" s="2">
         <v>40345</v>
@@ -1971,7 +1971,7 @@
     </row>
     <row r="51" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B51" s="2">
         <v>40403</v>
@@ -2001,7 +2001,7 @@
     </row>
     <row r="52" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B52" s="2">
         <v>40437</v>
@@ -2031,7 +2031,7 @@
     </row>
     <row r="53" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B53" s="2">
         <v>40465</v>
@@ -2061,7 +2061,7 @@
     </row>
     <row r="54" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B54" s="2">
         <v>40527</v>
@@ -2091,7 +2091,7 @@
     </row>
     <row r="55" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B55" s="2">
         <v>40549</v>
@@ -2121,7 +2121,7 @@
     </row>
     <row r="56" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B56" s="2">
         <v>40598</v>
@@ -2151,7 +2151,7 @@
     </row>
     <row r="57" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B57" s="2">
         <v>40659</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="58" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B58" s="2">
         <v>40723</v>
@@ -2211,7 +2211,7 @@
     </row>
     <row r="59" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B59" s="2">
         <v>40779</v>
@@ -2230,12 +2230,12 @@
       <c r="H59" s="9"/>
       <c r="I59" s="9"/>
       <c r="J59" s="19" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B60" s="2">
         <v>40848</v>
@@ -2257,7 +2257,7 @@
     </row>
     <row r="61" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B61" s="2">
         <v>40864</v>
@@ -2273,7 +2273,7 @@
     </row>
     <row r="62" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B62" s="2">
         <v>40238</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="63" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B63" s="2">
         <v>40281</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="64" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B64" s="2">
         <v>40316</v>
@@ -2363,7 +2363,7 @@
     </row>
     <row r="65" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B65" s="2">
         <v>40345</v>
@@ -2393,7 +2393,7 @@
     </row>
     <row r="66" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B66" s="2">
         <v>40403</v>
@@ -2423,7 +2423,7 @@
     </row>
     <row r="67" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B67" s="2">
         <v>40437</v>
@@ -2449,7 +2449,7 @@
     </row>
     <row r="68" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B68" s="2">
         <v>40465</v>
@@ -2475,7 +2475,7 @@
     </row>
     <row r="69" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B69" s="2">
         <v>40527</v>
@@ -2501,7 +2501,7 @@
     </row>
     <row r="70" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B70" s="2">
         <v>40549</v>
@@ -2531,7 +2531,7 @@
     </row>
     <row r="71" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B71" s="2">
         <v>40598</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="72" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B72" s="2">
         <v>40659</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="73" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B73" s="2">
         <v>40723</v>
@@ -2621,7 +2621,7 @@
     </row>
     <row r="74" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B74" s="2">
         <v>40779</v>
@@ -2651,7 +2651,7 @@
     </row>
     <row r="75" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B75" s="2">
         <v>40848</v>
@@ -2673,7 +2673,7 @@
     </row>
     <row r="76" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B76" s="2">
         <v>40864</v>
@@ -2695,7 +2695,7 @@
     </row>
     <row r="77" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B77" s="2">
         <v>40238</v>
@@ -2725,7 +2725,7 @@
     </row>
     <row r="78" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B78" s="2">
         <v>40281</v>
@@ -2755,7 +2755,7 @@
     </row>
     <row r="79" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B79" s="2">
         <v>40316</v>
@@ -2785,7 +2785,7 @@
     </row>
     <row r="80" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B80" s="2">
         <v>40345</v>
@@ -2815,7 +2815,7 @@
     </row>
     <row r="81" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B81" s="2">
         <v>40403</v>
@@ -2845,7 +2845,7 @@
     </row>
     <row r="82" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B82" s="2">
         <v>40437</v>
@@ -2875,7 +2875,7 @@
     </row>
     <row r="83" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B83" s="2">
         <v>40465</v>
@@ -2905,7 +2905,7 @@
     </row>
     <row r="84" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B84" s="2">
         <v>40527</v>
@@ -2935,7 +2935,7 @@
     </row>
     <row r="85" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B85" s="2">
         <v>40549</v>
@@ -2965,7 +2965,7 @@
     </row>
     <row r="86" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B86" s="2">
         <v>40598</v>
@@ -2995,7 +2995,7 @@
     </row>
     <row r="87" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B87" s="2">
         <v>40659</v>
@@ -3025,7 +3025,7 @@
     </row>
     <row r="88" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B88" s="2">
         <v>40723</v>
@@ -3055,7 +3055,7 @@
     </row>
     <row r="89" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B89" s="2">
         <v>40779</v>
@@ -3085,7 +3085,7 @@
     </row>
     <row r="90" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B90" s="2">
         <v>40848</v>
@@ -3107,7 +3107,7 @@
     </row>
     <row r="91" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B91" s="2">
         <v>40864</v>

</xml_diff>